<commit_message>
add TEA and LCA to system C
</commit_message>
<xml_diff>
--- a/exposan/co2_sorbent/data/impact_items.xlsx
+++ b/exposan/co2_sorbent/data/impact_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD_CEE/coding/cloned_packages/EXPOsan/exposan/co2_sorbent/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC204C2-6B02-FA40-8ACF-46E0E945F29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC4015C-8D71-0244-B135-73DAA695293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19180" yWindow="3240" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="1200" yWindow="500" windowWidth="50000" windowHeight="28300" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
   <si>
     <t>ecoinvent 3</t>
   </si>
@@ -107,6 +107,21 @@
   </si>
   <si>
     <t>market group for electricity, low voltage</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>ALF</t>
+  </si>
+  <si>
+    <t>calculate LCA for ALF by adjusting the ALF amount in the code and assuming its CI as 1</t>
   </si>
 </sst>
 </file>
@@ -479,19 +494,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.5" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.6640625" style="2"/>
   </cols>
   <sheetData>
@@ -552,6 +567,37 @@
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -561,16 +607,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE2E960-887B-1E49-80AF-9619BDC224B9}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
@@ -681,10 +728,50 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
update CO2ElectrolyzerSystem and LCA data
</commit_message>
<xml_diff>
--- a/exposan/co2_sorbent/data/impact_items.xlsx
+++ b/exposan/co2_sorbent/data/impact_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiananfeng/Desktop/PhD_CEE/coding/cloned_packages/EXPOsan/exposan/co2_sorbent/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC4015C-8D71-0244-B135-73DAA695293B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B598CD0C-F099-1945-B9B5-320CA540217E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="500" windowWidth="50000" windowHeight="28300" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
+    <workbookView xWindow="4000" yWindow="500" windowWidth="22920" windowHeight="28300" activeTab="1" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66379A7A-E84B-1346-816F-577916F7D6A6}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE2E960-887B-1E49-80AF-9619BDC224B9}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,15 +657,15 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>0.70378750999999995</v>
+        <v>0.70357913000000005</v>
       </c>
       <c r="D2" s="2">
         <f>C2*0.9</f>
-        <v>0.63340875899999993</v>
+        <v>0.63322121700000011</v>
       </c>
       <c r="E2" s="2">
         <f>C2*1.1</f>
-        <v>0.77416626099999997</v>
+        <v>0.7739370430000001</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>1</v>
@@ -683,15 +683,15 @@
         <v>10</v>
       </c>
       <c r="C3" s="2">
-        <v>6.6032741000000006E-2</v>
+        <v>6.5877932E-2</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D4" si="0">C3*0.9</f>
-        <v>5.9429466900000005E-2</v>
+        <v>5.9290138800000003E-2</v>
       </c>
       <c r="E3" s="2">
         <f t="shared" ref="E3:E4" si="1">C3*1.1</f>
-        <v>7.2636015100000006E-2</v>
+        <v>7.2465725200000011E-2</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>1</v>
@@ -709,15 +709,15 @@
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>0.11945807</v>
+        <v>0.1194374</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>0.107512263</v>
+        <v>0.10749366</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>0.131403877</v>
+        <v>0.13138114000000001</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>1</v>

</xml_diff>